<commit_message>
Malta dei um commit!
Updated checklist com cores!
</commit_message>
<xml_diff>
--- a/sd_checklist_meta2.xlsx
+++ b/sd_checklist_meta2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raul/Home/Git/SDIST/projeto_meta_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josphze\Desktop\SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB9790F-7E8D-044B-BC5E-A02A9F605344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F888AE-809B-431C-BA5E-31846D5E7C00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="27820" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-21" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>REST</t>
   </si>
@@ -178,13 +178,25 @@
   </si>
   <si>
     <t>Utilização em smartphone ou tablet (2pts)</t>
+  </si>
+  <si>
+    <t>Mudar para a consola de administração</t>
+  </si>
+  <si>
+    <t>Por Implementar</t>
+  </si>
+  <si>
+    <t>Implementado</t>
+  </si>
+  <si>
+    <t>Testado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -208,8 +220,16 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +239,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,7 +317,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,25 +337,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,6 +445,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFF9933"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -775,25 +834,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="121" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="121" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="75.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:70" s="5" customFormat="1">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -801,7 +860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:70" s="5" customFormat="1">
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -809,7 +868,7 @@
         <v>2017987654</v>
       </c>
     </row>
-    <row r="5" spans="1:70" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:70" s="5" customFormat="1">
       <c r="A5" s="5">
         <f>A6+A21+A25+A31</f>
         <v>100</v>
@@ -1074,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="BO5" s="5">
-        <f t="shared" ref="BO5:CT5" si="2">BO6+BO21+BO25+BO31+BO36+BO41</f>
+        <f t="shared" ref="BO5:BR5" si="2">BO6+BO21+BO25+BO31+BO36+BO41</f>
         <v>0</v>
       </c>
       <c r="BP5" s="5">
@@ -1090,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="A6" s="1">
         <f>SUM(A7:A20)</f>
         <v>57</v>
@@ -1371,161 +1430,180 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A9" s="9">
         <v>5</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A10" s="9">
         <v>5</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A11" s="9">
         <v>5</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A12" s="9">
         <v>5</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A13" s="9">
         <v>5</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="14" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A14" s="9">
         <v>7</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A15" s="9">
         <v>5</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="16" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A16" s="9">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+    <row r="17" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A17" s="9">
         <v>5</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>0</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A18" s="7">
+        <v>0</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>0</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A19" s="9">
+        <v>0</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>0</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A20" s="9">
+        <v>0</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="A21" s="1">
         <f>SUM(A22:A24)</f>
         <v>15</v>
@@ -1806,40 +1884,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+    <row r="22" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A22" s="9">
         <v>5</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+    <row r="23" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A23" s="9">
         <v>5</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+    <row r="24" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A24" s="9">
         <v>5</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="A25" s="1">
         <f>SUM(A26:A30)</f>
         <v>20</v>
@@ -2120,62 +2198,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+    <row r="26" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A26" s="9">
         <v>5</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+    <row r="27" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A27" s="9">
         <v>5</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+    <row r="28" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A28" s="9">
         <v>5</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+    <row r="29" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A29" s="9">
         <v>5</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>0</v>
-      </c>
-      <c r="B30" s="4" t="s">
+    <row r="30" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A30" s="9">
+        <v>0</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="A31" s="1">
         <f>SUM(A32:A35)</f>
         <v>8</v>
@@ -2440,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="BO31" s="1">
-        <f t="shared" ref="BO31:CT31" si="11">SUM(BO32:BO35)</f>
+        <f t="shared" ref="BO31:BR31" si="11">SUM(BO32:BO35)</f>
         <v>0</v>
       </c>
       <c r="BP31" s="1">
@@ -2456,51 +2534,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+    <row r="32" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A32" s="7">
         <v>2</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+    <row r="33" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A33" s="7">
         <v>2</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+    <row r="34" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A34" s="7">
         <v>2</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+    <row r="35" spans="1:70" s="3" customFormat="1" ht="18.75">
+      <c r="A35" s="7">
         <v>2</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="B36" s="2" t="s">
         <v>10</v>
       </c>
@@ -2777,27 +2855,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B37" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B38" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B39" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B40" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="B41" s="2" t="s">
         <v>12</v>
       </c>
@@ -3074,32 +3152,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B42" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B43" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B44" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B45" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:70" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:70" s="3" customFormat="1" ht="18.75">
       <c r="B46" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:70" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:70" s="1" customFormat="1" ht="18.75">
       <c r="B47" s="2" t="s">
         <v>17</v>
       </c>
@@ -3378,5 +3456,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>